<commit_message>
correctly doing knn now
</commit_message>
<xml_diff>
--- a/assignment-1/results.xlsx
+++ b/assignment-1/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chaya\ATU Galway\gbui-projects-2024\assignment-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F04B1596-E116-4E5A-B257-6B5320218F8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF87FB5-B029-4C4A-9205-CC6EC53AA72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{99926DC4-29C1-42AE-BBBD-093A032E451F}"/>
   </bookViews>
@@ -36,27 +36,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
-  <si>
-    <t>fold 1</t>
-  </si>
-  <si>
-    <t>c 5, gamma 10, rbf</t>
-  </si>
-  <si>
-    <t>c 5, gamma 1, rbf</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="16">
   <si>
     <t>4 vars</t>
   </si>
   <si>
-    <t>4+ vars</t>
-  </si>
-  <si>
     <t>6 vars</t>
-  </si>
-  <si>
-    <t>c 2, gamma 1, rbf</t>
   </si>
   <si>
     <t>Logistic</t>
@@ -69,6 +54,36 @@
   </si>
   <si>
     <t>SVM</t>
+  </si>
+  <si>
+    <t>k = 1</t>
+  </si>
+  <si>
+    <t>{'svc__C': 5, 'svc__gamma': 10, 'svc__kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>{'svc__C': 1, 'svc__gamma': 10, 'svc__kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>5 vars</t>
+  </si>
+  <si>
+    <t>For trial 3</t>
+  </si>
+  <si>
+    <t>k = 3</t>
+  </si>
+  <si>
+    <t>{'svc__C': 5, 'svc__gamma': 1, 'svc__kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>{'svc__C': 2, 'svc__gamma': 10, 'svc__kernel': 'rbf'}</t>
+  </si>
+  <si>
+    <t>3 vars</t>
+  </si>
+  <si>
+    <t>less vars = more execution time in polynomial for svm - 3 vars</t>
   </si>
 </sst>
 </file>
@@ -251,16 +266,16 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="4"/>
                 <c:pt idx="0">
-                  <c:v>0.58840579710144902</c:v>
+                  <c:v>0.55463768115942003</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.76594202898550701</c:v>
+                  <c:v>0.76463768115941999</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.76659948945317724</c:v>
+                  <c:v>0.77873443971283163</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.78782608695652101</c:v>
+                  <c:v>0.77492753623188348</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1128,6 +1143,50 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>600075</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>391432</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>162603</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D6506C68-2B72-ACD5-897F-202C5C480D56}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8391525" y="1971675"/>
+          <a:ext cx="6496957" cy="4858428"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1428,10 +1487,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EED96714-06E7-4735-AE9A-FA70E0092CD8}">
-  <dimension ref="A3:J9"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A2:L10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O26" sqref="O26"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1442,165 +1502,182 @@
     <col min="5" max="5" width="13.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="G2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="B4" s="1">
-        <v>0.59347826086956501</v>
+        <v>0.51884057971014497</v>
       </c>
       <c r="C4" s="1">
-        <v>0.76231884057971</v>
+        <v>0.77826086956521701</v>
       </c>
       <c r="D4" s="1">
-        <v>0.78177452990554297</v>
+        <v>0.80304546436978996</v>
       </c>
       <c r="E4" s="1">
-        <v>0.80144927536231803</v>
+        <v>0.80652173913043401</v>
       </c>
       <c r="G4" t="s">
         <v>0</v>
       </c>
       <c r="H4" t="s">
-        <v>1</v>
+        <v>6</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
       <c r="B5" s="1">
-        <v>0.58913043478260796</v>
+        <v>0.59202898550724603</v>
       </c>
       <c r="C5" s="1">
-        <v>0.74710144927536204</v>
+        <v>0.77318840579710102</v>
       </c>
       <c r="D5" s="1">
-        <v>0.74189375485574405</v>
+        <v>0.78226141866591803</v>
       </c>
       <c r="E5" s="1">
-        <v>0.74710144927536204</v>
+        <v>0.78188405797101401</v>
       </c>
       <c r="G5" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" t="s">
-        <v>2</v>
+        <v>6</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
       <c r="B6" s="1">
-        <v>0.602173913043478</v>
+        <v>0.59565217391304304</v>
       </c>
       <c r="C6" s="1">
-        <v>0.8</v>
+        <v>0.75797101449275295</v>
       </c>
       <c r="D6" s="1">
-        <v>0.77187290071207804</v>
+        <v>0.76679693204586696</v>
       </c>
       <c r="E6" s="1">
-        <v>0.83260869565217299</v>
+        <v>0.74420289855072397</v>
       </c>
       <c r="G6" t="s">
-        <v>0</v>
+        <v>9</v>
       </c>
       <c r="H6" t="s">
-        <v>2</v>
-      </c>
-      <c r="J6" t="s">
-        <v>4</v>
+        <v>11</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
       <c r="B7" s="1">
-        <v>0.52101449275362299</v>
+        <v>0.54710144927536197</v>
       </c>
       <c r="C7" s="1">
-        <v>0.75869565217391299</v>
+        <v>0.76376811594202898</v>
       </c>
       <c r="D7" s="1">
-        <v>0.75423274859950096</v>
+        <v>0.78782661269123599</v>
       </c>
       <c r="E7" s="1">
-        <v>0.77898550724637605</v>
+        <v>0.78913043478260803</v>
       </c>
       <c r="G7" t="s">
         <v>0</v>
       </c>
       <c r="H7" t="s">
-        <v>1</v>
-      </c>
-      <c r="J7" t="s">
-        <v>3</v>
+        <v>6</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
       <c r="B8" s="1">
-        <v>0.63623188405797104</v>
+        <v>0.51956521739130401</v>
       </c>
       <c r="C8" s="1">
-        <v>0.76159420289854995</v>
+        <v>0.75</v>
       </c>
       <c r="D8" s="1">
-        <v>0.78322351319301997</v>
+        <v>0.75374177079134697</v>
       </c>
       <c r="E8" s="1">
-        <v>0.77898550724637605</v>
+        <v>0.75289855072463696</v>
       </c>
       <c r="G8" t="s">
-        <v>0</v>
+        <v>14</v>
       </c>
       <c r="H8" t="s">
-        <v>6</v>
-      </c>
-      <c r="J8" t="s">
-        <v>5</v>
+        <v>11</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9">
         <f>AVERAGE(B4:B8)</f>
-        <v>0.58840579710144902</v>
+        <v>0.55463768115942003</v>
       </c>
       <c r="C9">
         <f t="shared" ref="C9:E9" si="0">AVERAGE(C4:C8)</f>
-        <v>0.76594202898550701</v>
+        <v>0.76463768115941999</v>
       </c>
       <c r="D9">
         <f t="shared" si="0"/>
-        <v>0.76659948945317724</v>
+        <v>0.77873443971283163</v>
       </c>
       <c r="E9">
         <f t="shared" si="0"/>
-        <v>0.78782608695652101</v>
+        <v>0.77492753623188348</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="L10" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>